<commit_message>
Avances al 17 de Marzo
Revisión de Audios de pruebas. 8 de 12
</commit_message>
<xml_diff>
--- a/resultado de test de usabilidad.xlsx
+++ b/resultado de test de usabilidad.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-27040" yWindow="600" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SUSALUD" sheetId="1" r:id="rId1"/>
     <sheet name="Gestores" sheetId="2" r:id="rId2"/>
     <sheet name="Ciudadanos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>SUSALUD #1</t>
   </si>
@@ -40,15 +40,6 @@
     <t>SUSALUD #3</t>
   </si>
   <si>
-    <t>SUSALUD #4</t>
-  </si>
-  <si>
-    <t>SUSALUD #5</t>
-  </si>
-  <si>
-    <t>SUSALUD #6</t>
-  </si>
-  <si>
     <t>Tarea 1</t>
   </si>
   <si>
@@ -133,15 +124,230 @@
     <t>Ciudadano #5</t>
   </si>
   <si>
-    <t>Ciudadano #6</t>
+    <t>Gestor #6</t>
+  </si>
+  <si>
+    <t>No tuvo problemas en entender el proposito de cada pantalla.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arreglar problemas de links. Cambio de labels para mejor entendimiento. Elegir telefono y email como medio preferido. Solicitudes que se resuelven rapido, como colocarlo? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concepto 'quejosos frecuentes' util pero necesita capacitación. Validación con DNI esta bien. Datos del paciente con DNI esta bien. TA BONITO. Radio Button de Email y Telefono arreglar la forma de marcación. Que la solicitud llegue a la IPRESS es mejor a que vaya directo a SUSALUD, esta bien. Historico y Gestión esta bien separados, se entiende bien. Estadisticas le gusto que fuera con graficos.  </t>
+  </si>
+  <si>
+    <t>Gestión de Solicitudes</t>
+  </si>
+  <si>
+    <t>Estadisticas</t>
+  </si>
+  <si>
+    <t>Historico de Solicitudes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Busco opción Inicio. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Link Estadisticas no funciona</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Apretar 2 veces al boton hacen que opción aparezca y desaparezca. Seleccionar archivo explicar un poco más. Se podria elegir Telefono Y email. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Paso 4 deberia ser Hoja Resumen de la Solicitud</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Estado 'NUEVO' no es entendible al comienzo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">No busco en los detalles. </t>
+    </r>
+  </si>
+  <si>
+    <t>Miedo en la interacción. Tipo de Solicitud no la vio. No termino la cantidad de pasos para Nueva solicitud. Separación entre Vigentes en Gestión de Solicitudes e Historico esta bien. Identificación es necesaria y esta bien. Estado 'NUEVO' no se entiende tan mal.</t>
+  </si>
+  <si>
+    <t>Necesito un poco de guia para interactuar con la herramienta por miedo, pero entendio bien los objetivos de las pantallas.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dice 'Esta bien y que le hubiera servido'. Le parece </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interesante</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Gran ayuda.</t>
+    </r>
+  </si>
+  <si>
+    <t>Estadisticas en barras.</t>
+  </si>
+  <si>
+    <t>Indico que hay una normativa de clasificacion de reclamos que se reflejan en indicadores. No cambio nada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No interactuo con las tarjetas. Detallo en forma no especifica los reclamos que conoce. </t>
+  </si>
+  <si>
+    <t>Propuesta: Situación actual</t>
+  </si>
+  <si>
+    <t>Propuesta: Servicio comprometido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No todos quieren identificarse, considerar anonimos. Especificar servicio de donde ocurrio el problema. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No quiso interactuar solo con el sistema.  Magnitud de la queja ya que hay pesos diferentes de quejas. </t>
+  </si>
+  <si>
+    <t>Conto experiencia de 'vigilancia de rumores' para poner rumores anonimos en el sistema. Personas no se quejan por miedo a represalias. Como se considerarian los reclamos internos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parentezco con solicitante. </t>
+  </si>
+  <si>
+    <t>Busca Inicio, si empieza con Nueva Solicitud piensan que es poner su propio DNI. Creen que solo es la información que esta a primera vista, no hacen scroll down. Entiende el concepto del Nuevo pero parece que no lo termina de convencer. Salir del lightbox es complicado y buscan salir apretando fuera nomas.</t>
+  </si>
+  <si>
+    <t>Evidencia esta bien. Detalle de la solicitud esta interesante. Más filtros por DIRIS o DISAS.</t>
+  </si>
+  <si>
+    <t>Gestion de Solicitudes</t>
+  </si>
+  <si>
+    <t>No pudo revisar la clasificación propuesta de reclamos</t>
+  </si>
+  <si>
+    <t>Reviso cada categoria e item, no comprendio forma de uso de Trello, agrego Cobros Indebidos en Problemas de Seguro, dentro de problemas de información agrego Tarifarios No Visibles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derivación de solicitudes para IPRESS de origen de solicitud. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seria bueno que el paciente pueda responder a las respuestas de los pasos hechos. Propuesta de estado nuevo 'No Solucionable'. Quejas de parte del usuario interno hacia los ciudadanos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entendio pantalla inicial de Nueva Solicitud. Entendio Gestion de Reclamos. Estadisticas le gusto. </t>
+  </si>
+  <si>
+    <t>Reviso cada categoria e item. Considera que de infraestructura no se dan reclamos. Cambio de medico tratante no se quejan. Todos se quejarian de Demora reconsiderar esta parte.</t>
+  </si>
+  <si>
+    <t>Problemas con elegir la fecha en el calendario. Buscar por nombre, nombre de que? Cambiar IPRESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicio del cual me estoy quejando. Poder quejarse por un ciudadano desconocido. Tipificar el reclamo. Fecha para cuando se deberia resolver el reclamo. En estadisitcias colocar el # total de reclamos. Identificar que medico tiene mas quejas. Descargar el descargo de la solicitud. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial para explicar la diferencia entre tipos de solicitudes. Chat interno para hacer las consultas. Poner cuantos dias se demoraran en responder, no es suficiente. Filtros para las tablas de solicitudes. </t>
+  </si>
+  <si>
+    <t>Comprendio en general todo bien. En buscar centro de salud no entendio buscar que cosa</t>
+  </si>
+  <si>
+    <t>Miedo a interactuar con la computadora.</t>
+  </si>
+  <si>
+    <t>Le parece interesante ya que le parece como una forma de comunicarse con su IPRESS. Solicitudes Vigentes y Pasadas entendio bien</t>
+  </si>
+  <si>
+    <t>Comprendio bien las pantallas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitudes bien recibido. Le parece interesante. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -183,6 +389,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -451,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G12"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +672,7 @@
     <col min="2" max="7" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -473,82 +682,73 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="96" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="112" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="112" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -558,10 +758,196 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F10"/>
+  <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="240" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,133 +958,73 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="208" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="304" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="7" width="16.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avances al 20 de Marzo
Todas mis correcciones hechas al 20 de marzo. Faltan correcciones
pequeñas que dio ccc hasta parte de SUSALUD. Falta terminar resultados,
discusión, recomendaciones y conclusiones
</commit_message>
<xml_diff>
--- a/resultado de test de usabilidad.xlsx
+++ b/resultado de test de usabilidad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>SUSALUD #1</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t xml:space="preserve">Solicitudes bien recibido. Le parece interesante. </t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -947,7 +950,7 @@
   <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,6 +986,9 @@
       <c r="E3" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1018,6 +1024,9 @@
       <c r="E7" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="304" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1025,6 +1034,12 @@
       </c>
       <c r="B8" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avances en trabajo final hasta el 21 de marzo
Se agregaron resultados de los test de usabilidad
</commit_message>
<xml_diff>
--- a/resultado de test de usabilidad.xlsx
+++ b/resultado de test de usabilidad.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27040" yWindow="600" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUSALUD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
   <si>
     <t>SUSALUD #1</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Comentarios</t>
   </si>
   <si>
-    <t>Flujo seguido</t>
-  </si>
-  <si>
     <t>Cambios sugeridos</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>Correcta en 7. 2 pantallas no fueron vistas</t>
-  </si>
-  <si>
-    <t>Flujo planteado</t>
   </si>
   <si>
     <t>Gestor #1</t>
@@ -335,6 +329,75 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vio boton de Detalle. Les gusta la idea de un sistema centralizado. Formalizar los IBOs. Se evitaria papeleo. Interactivo y esta bien. Semaforización esta bien que sea automatico. Ven importante el sistema para el monitoreo. Amigable y super interesante. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No vio 'Gestión de Solicitudes'. Se tiene que hacer diferenciación en webs para distintos usuarios. Interesante ver el perfil de la persona. Ver la hoja de respuesta del reclamo. </t>
+  </si>
+  <si>
+    <t>Como manejar los IBOs</t>
+  </si>
+  <si>
+    <t>Le parecio claro por las agrupaciones</t>
+  </si>
+  <si>
+    <t>Hubo problemas con textos de algunas paginas pero entendio las paginas que reviso sin problema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problema con la fecha de nacimiento, no se puede elegir bien y no permite escribir la fecha. Los colores de la semaforización no se deja a entender en el tiempo, da a entender que es por estado. Deberia ponerse ambas formas de ser contactado. Orden del resumen parece que esta un poco confuso ya que piensan que deben colocar de nuevo la info. Cual fue la respuesta ante el reclamo (colocar la carta de respuesta). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le gusta la idea de poder reclamar por un dependiente. Esperan que siempre les llegue una copia al mail. 'Estadisticas' solo no se entiende de que son las estadisticas. Le parece interesante. Entendio bien parte de mis solicitudes, actuales y pasadas. Paleta de colores agradable. </t>
+  </si>
+  <si>
+    <t>Nueva Solicitud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombres en labels aún es confuso, sobre todo 'Ver situación actual en centro de salud' (no se entiende de que), estadisticas (de que?). En estadisticas, lista de centro de salud seria muy larga, cambiar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alineación de iconos confuso. Pantalla de inicio? Orden del menu es confuso. Le gusta saber cuantos pasos son de la nueva solicitud. Colocar domicilio nuevo es tedioso, explicar porque se necesita el actualizado. Como saber si eres el ciudadano afectado? Explicar que es el ciudadano afectado. </t>
+  </si>
+  <si>
+    <t>Paso 2. Buscar por nombre, nombre de que? Tipo de solicitud esta mal posicionada. Botones con mismo peso. Que tipo de archivos puedo adjuntar? Resumen tiene muchos datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dar modelos de solicitudes escritas para que el usuario piense menos y de mejor información. Cambiar el lenguaje para alguien que no es muy inteligente. Resumen de mis solicitudes es necesario. </t>
+  </si>
+  <si>
+    <t>Tuvo dificultades por textos en titulos, recomendo como solucionarlo. Botones todos del mismo color da la impresión que tienen el mismo peso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derivación de solicitudes para hospital de origen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semaforización esta bien. Apelación esta bien ya que sino SUSALUD hace el trabajo de la IPRESS. Solucionados y vigentes esta bien que este separado. Historico por tiempo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buena reacción ante Solicitudes. Sistema le parece muy bien. Tipo 'No Solucionable' deberia agregarse. </t>
+  </si>
+  <si>
+    <t>Sin problemas para entender</t>
+  </si>
+  <si>
+    <t>Referencia a Elvia Campos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorización no se entendio, se tuvo que explicar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estadisticas por IPRESS le parece bien, pero para los gestores, no cree que los ciudadanos lo entenderian. Encontro el boton de detalle. Sistma esta simpatico. Filtros no quedaban muy claros. </t>
+  </si>
+  <si>
+    <t>Comprende sin problemas las pantallas.</t>
+  </si>
+  <si>
+    <t>No planteo cambios grandes, solo refinar los titulos para mejor entendimiento y mejores graficos para ciudadanos</t>
+  </si>
+  <si>
+    <t>Hablo sobre nueva clasificación que ya esta siendo aprobada</t>
   </si>
 </sst>
 </file>
@@ -663,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D12"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,70 +751,125 @@
     </row>
     <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="192" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -763,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,48 +893,51 @@
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -824,19 +945,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -844,99 +968,114 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="288" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -949,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,85 +1100,124 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="208" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="304" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="304" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios al 21 de Marzo
Cambios al 21 de marzo antes de reunion con ccc. esperando correcciones
de el.
</commit_message>
<xml_diff>
--- a/resultado de test de usabilidad.xlsx
+++ b/resultado de test de usabilidad.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SUSALUD" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>SUSALUD #1</t>
   </si>
@@ -729,7 +729,7 @@
   <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1139,6 +1139,9 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
       <c r="C4" t="s">
         <v>74</v>
       </c>
@@ -1149,6 +1152,9 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>

</xml_diff>